<commit_message>
results from XLNET-based segmenter
</commit_message>
<xml_diff>
--- a/outputs/20250601_185319/message_report/parsed_DJIFlightRecord_2025-05-12_[08-01-12]_message.xlsx
+++ b/outputs/20250601_185319/message_report/parsed_DJIFlightRecord_2025-05-12_[08-01-12]_message.xlsx
@@ -3149,11 +3149,7 @@
           <t>RC signal lost. Aircraft will follow preset action for lost signal.</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
+      <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr">
         <is>
           <t>E4</t>
@@ -3209,11 +3205,7 @@
           <t>RC signal lost. Aircraft will follow preset action for lost signal.</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
+      <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr">
         <is>
           <t>E4</t>
@@ -3599,11 +3591,7 @@
           <t>RC signal lost. Aircraft will follow preset action for lost signal.</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>medium</t>
-        </is>
-      </c>
+      <c r="E106" t="inlineStr"/>
       <c r="F106" t="inlineStr">
         <is>
           <t>E4</t>

</xml_diff>